<commit_message>
changes in connection string key names for better understanding
</commit_message>
<xml_diff>
--- a/config_dummy.xlsx
+++ b/config_dummy.xlsx
@@ -26,13 +26,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
-    <t>localDb</t>
+    <t>connStr</t>
   </si>
   <si>
-    <t>conStr</t>
+    <t>appDbConStr</t>
   </si>
   <si>
-    <t>connStr</t>
+    <t>reportsConStr</t>
   </si>
 </sst>
 </file>
@@ -405,28 +405,29 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="74.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>